<commit_message>
Fixed Bar formatting Issue
</commit_message>
<xml_diff>
--- a/documents/Published/GanttChart/GanttChartByMAQSoftwareChecklist.xlsx
+++ b/documents/Published/GanttChart/GanttChartByMAQSoftwareChecklist.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PowerBI\PowerBI-visuals\documents\Published\GanttChart\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\New folder\documents\Published\GanttChart\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86844A70-3D25-4F24-9412-5045992FFB9E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10215" xr2:uid="{15650058-D9E1-4E2D-A421-D272244BB495}"/>
   </bookViews>
@@ -973,8 +974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AD304B0-4792-43AB-9D20-CD62C2AB01B6}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>